<commit_message>
Se crea la primera implementacion del modelo
</commit_message>
<xml_diff>
--- a/Catalogo.xlsx
+++ b/Catalogo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/258fc4206f515148/Documentos/Especialización analitica y ciencia de datos/Code/Machine Learning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/258fc4206f515148/Documentos/Especialización analitica y ciencia de datos/Code/Machine Learning/jobML/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="56" documentId="11_45B171ADD3705716AB793F11595ED87656CEDE80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D771CE5-6FCF-4035-A802-23FCE88010D2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1905" yWindow="1905" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>